<commit_message>
First Test Suite update
</commit_message>
<xml_diff>
--- a/bin/com/packagename/xlsmain/Suite.xlsx
+++ b/bin/com/packagename/xlsmain/Suite.xlsx
@@ -465,7 +465,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,7 +505,7 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -516,7 +516,7 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -527,7 +527,7 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
True Color excel updates
</commit_message>
<xml_diff>
--- a/bin/com/packagename/xlsmain/Suite.xlsx
+++ b/bin/com/packagename/xlsmain/Suite.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Runmode</t>
   </si>
@@ -44,85 +44,61 @@
     <t>TSID</t>
   </si>
   <si>
-    <t>Product_Verification</t>
-  </si>
-  <si>
-    <t>AddToCart_Verification</t>
-  </si>
-  <si>
-    <t>Order_Module</t>
-  </si>
-  <si>
-    <t>EvolveMoney_Module</t>
-  </si>
-  <si>
-    <t>GiftVoucher_Module</t>
-  </si>
-  <si>
-    <t>Hamper_Module</t>
-  </si>
-  <si>
-    <t>Browser_Verification</t>
-  </si>
-  <si>
-    <t>Registeration_Verification</t>
-  </si>
-  <si>
-    <t>Subscription_Module</t>
-  </si>
-  <si>
-    <t>Form_Verification</t>
-  </si>
-  <si>
-    <t>Link_Verification</t>
-  </si>
-  <si>
-    <t>Gift Voucher based Test Cases</t>
-  </si>
-  <si>
-    <t>Navigation based Test Cases execute</t>
-  </si>
-  <si>
-    <t>All Products based Test Cases execute</t>
-  </si>
-  <si>
-    <t>Add all type of product based Test Cases execute</t>
-  </si>
-  <si>
-    <t>Order status  based Test Cases execute</t>
-  </si>
-  <si>
-    <t>Evolve money based Test Cases execute</t>
-  </si>
-  <si>
-    <t>Referal based Test Cases execute</t>
-  </si>
-  <si>
-    <t>Hamper_Module based Test Cases</t>
-  </si>
-  <si>
-    <t>Subscription_Module based Test Cases</t>
-  </si>
-  <si>
-    <t>Form_Verification based Test Cases</t>
-  </si>
-  <si>
-    <t>Link_Verification based Test Cases</t>
-  </si>
-  <si>
-    <t>Browser_Verification based Test Cases</t>
-  </si>
-  <si>
-    <t>Registeration_Verification based Test Cases</t>
-  </si>
-  <si>
-    <t>Referral _Module</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
     <t>All type of login execution</t>
+  </si>
+  <si>
+    <t>Teacher_Verification</t>
+  </si>
+  <si>
+    <t>Parent_Verification</t>
+  </si>
+  <si>
+    <t>Student_Verification</t>
+  </si>
+  <si>
+    <t>Class_Verification</t>
+  </si>
+  <si>
+    <t>User_Verification</t>
+  </si>
+  <si>
+    <t>Resources_Verification</t>
+  </si>
+  <si>
+    <t>SimpleSearch_Verification</t>
+  </si>
+  <si>
+    <t>AdvanceSearch_Verification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teacher Module Testing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parent Module Testing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student Module Testing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Module Testing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advance  Search Module Testing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simple Search  Module Testing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resources Module Testing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Class Verification Module Testing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Page UI and Navigation verification testing </t>
   </si>
 </sst>
 </file>
@@ -462,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +467,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -502,142 +478,98 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>